<commit_message>
Craete ExcelToJsonFileConverter + usint Tests
</commit_message>
<xml_diff>
--- a/src/Saturn72.FileConverters.Tests/Resources/some-data.xlsx
+++ b/src/Saturn72.FileConverters.Tests/Resources/some-data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t xml:space="preserve">A</t>
   </si>
@@ -52,9 +52,6 @@
     <t xml:space="preserve">2_2</t>
   </si>
   <si>
-    <t xml:space="preserve">2_3</t>
-  </si>
-  <si>
     <t xml:space="preserve">2_4</t>
   </si>
   <si>
@@ -70,9 +67,6 @@
     <t xml:space="preserve">3_4</t>
   </si>
   <si>
-    <t xml:space="preserve">4_1</t>
-  </si>
-  <si>
     <t xml:space="preserve">4_2</t>
   </si>
   <si>
@@ -85,9 +79,6 @@
     <t xml:space="preserve">5_1</t>
   </si>
   <si>
-    <t xml:space="preserve">5_2</t>
-  </si>
-  <si>
     <t xml:space="preserve">5_3</t>
   </si>
   <si>
@@ -110,9 +101,6 @@
   </si>
   <si>
     <t xml:space="preserve">7_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7_3</t>
   </si>
   <si>
     <t xml:space="preserve">7_4</t>
@@ -199,7 +187,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -209,10 +197,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -236,7 +220,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="A1:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -268,92 +252,84 @@
       <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="1" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="1" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="1" t="s">
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="C8" s="1"/>
+      <c r="D8" s="1" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
conversion for excel types
</commit_message>
<xml_diff>
--- a/src/Saturn72.FileConverters.Tests/Resources/some-data.xlsx
+++ b/src/Saturn72.FileConverters.Tests/Resources/some-data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t xml:space="preserve">A</t>
   </si>
@@ -34,73 +34,37 @@
     <t xml:space="preserve">D</t>
   </si>
   <si>
-    <t xml:space="preserve">1_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1_2</t>
-  </si>
-  <si>
     <t xml:space="preserve">1_3</t>
   </si>
   <si>
     <t xml:space="preserve">1_4</t>
   </si>
   <si>
-    <t xml:space="preserve">2_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2_2</t>
-  </si>
-  <si>
     <t xml:space="preserve">2_4</t>
   </si>
   <si>
-    <t xml:space="preserve">3_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3_2</t>
-  </si>
-  <si>
     <t xml:space="preserve">3_3</t>
   </si>
   <si>
     <t xml:space="preserve">3_4</t>
   </si>
   <si>
-    <t xml:space="preserve">4_2</t>
-  </si>
-  <si>
     <t xml:space="preserve">4_3</t>
   </si>
   <si>
     <t xml:space="preserve">4_4</t>
   </si>
   <si>
-    <t xml:space="preserve">5_1</t>
-  </si>
-  <si>
     <t xml:space="preserve">5_3</t>
   </si>
   <si>
     <t xml:space="preserve">5_4</t>
   </si>
   <si>
-    <t xml:space="preserve">6_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6_2</t>
-  </si>
-  <si>
     <t xml:space="preserve">6_3</t>
   </si>
   <si>
     <t xml:space="preserve">6_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7_2</t>
   </si>
   <si>
     <t xml:space="preserve">7_4</t>
@@ -124,19 +88,16 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="177"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="177"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="177"/>
     </font>
     <font>
       <sz val="10"/>
@@ -220,7 +181,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="A1:D8"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -243,93 +204,93 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="1" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
+      <c r="A3" s="1" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>12</v>
+      <c r="A4" s="1" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1"/>
-      <c r="B5" s="1" t="s">
-        <v>15</v>
+      <c r="B5" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>18</v>
+      <c r="A6" s="1" t="n">
+        <v>5.1</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>22</v>
+      <c r="A7" s="1" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>26</v>
+      <c r="A8" s="1" t="n">
+        <v>7.1</v>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>7</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>